<commit_message>
8 of 450 questins done
</commit_message>
<xml_diff>
--- a/src/asset/DSA-450.xlsx
+++ b/src/asset/DSA-450.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$C$481</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1844,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1854,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
-      <selection activeCell="B173" sqref="B173"/>
+    <sheetView tabSelected="1" topLeftCell="A324" workbookViewId="0">
+      <selection activeCell="C182" sqref="C182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3701,7 +3704,7 @@
         <v>172</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="21">
@@ -3723,7 +3726,7 @@
         <v>174</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="21">
@@ -3745,7 +3748,7 @@
         <v>176</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="21">
@@ -7375,5 +7378,6 @@
     <hyperlink ref="B2" r:id="rId446"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId447"/>
 </worksheet>
 </file>
</xml_diff>